<commit_message>
master_intern now comparable to excel datasource with ects
</commit_message>
<xml_diff>
--- a/backend/zulassung.xlsx
+++ b/backend/zulassung.xlsx
@@ -1,28 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhbi-my.sharepoint.com/personal/steven_michel_fhbi_onmicrosoft_com/Documents/7. Semester/2. Innovations-&amp; Projektmanagement/Projektarbeit/HSBI_Chatbot/backend/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhbi-my.sharepoint.com/personal/steven_michel_fhbi_onmicrosoft_com/Documents/B.Eng/7. Semester/2. Innovations-&amp; Projektmanagement/Projektarbeit/HSBI_Chatbot/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{531DFBDF-0543-4A2A-A4FF-3FDCFE07F64E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4830E394-FFB0-4CEC-9AB3-A9D9E223A9C3}"/>
+  <xr:revisionPtr revIDLastSave="302" documentId="8_{9D362DC0-2740-4FD3-9197-17AC54460654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E53E7371-9A4E-450A-837E-726B6EDB8719}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Allgemein" sheetId="1" r:id="rId1"/>
     <sheet name="Studiengänge" sheetId="2" r:id="rId2"/>
     <sheet name="Module" sheetId="3" r:id="rId3"/>
+    <sheet name="Modulzusammensetzung" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="471">
   <si>
     <t>Schlüssel</t>
   </si>
@@ -171,7 +188,7 @@
     <t>Berufspädagogik 2</t>
   </si>
   <si>
-    <t>Beschaffung, Produktion und Logistik</t>
+    <t>Beschaffung Produktion und Logistik</t>
   </si>
   <si>
     <t>Betriebssysteme</t>
@@ -324,7 +341,7 @@
     <t>Eingebettete Systeme in der Mechatronik</t>
   </si>
   <si>
-    <t>Eisenbahninfrastruktur (Fahrweg, Leit- und Sicherungstechnik)</t>
+    <t>Eisenbahninfrastruktur (Fahrweg Leit- und Sicherungstechnik)</t>
   </si>
   <si>
     <t>Electromobility</t>
@@ -393,6 +410,9 @@
     <t>English for Business and Engineering 1</t>
   </si>
   <si>
+    <t>English for Business und Engineering 2</t>
+  </si>
+  <si>
     <t>Erneuerbare und konventionelle Energieerzeugung</t>
   </si>
   <si>
@@ -864,7 +884,7 @@
     <t>Predictive Analytics</t>
   </si>
   <si>
-    <t>Product-Service ­Engineering – ­Einführung und Übersicht</t>
+    <t>Product-Service Engineering - Einführung und Übersicht</t>
   </si>
   <si>
     <t>Produktaufreinigung</t>
@@ -894,18 +914,33 @@
     <t>Projekt Automatisierungstechnik</t>
   </si>
   <si>
+    <t>Projekt Autonome Systeme und Robotik</t>
+  </si>
+  <si>
     <t>Projekt Data Science</t>
   </si>
   <si>
+    <t>Projekt Energie und Effizienz</t>
+  </si>
+  <si>
+    <t>Projekt Mechatronik</t>
+  </si>
+  <si>
     <t>Projekt Medizintechnik</t>
   </si>
   <si>
+    <t>Projekt Mobilität</t>
+  </si>
+  <si>
     <t>Projekt Nachhaltige Produkte und Prozesse</t>
   </si>
   <si>
     <t>Projektmanagement</t>
   </si>
   <si>
+    <t>Projektseminar (Angewandte Mathematik)</t>
+  </si>
+  <si>
     <t>Prozess- und Informationsmanagement Modul 1 Profilschwerpunkt (PSP)</t>
   </si>
   <si>
@@ -921,7 +956,7 @@
     <t>Rechnerarchitekturen</t>
   </si>
   <si>
-    <t>Rechnungwesen, Investition, Finanzierung und Steuern</t>
+    <t>Rechnungwesen Investition Finanzierung und Steuern</t>
   </si>
   <si>
     <t>Regelungs- und Automatisierungssysteme</t>
@@ -990,7 +1025,7 @@
     <t>Statik</t>
   </si>
   <si>
-    <t>Statik, Dynamik, Festigkeitslehre</t>
+    <t>Statik Dynamik Festigkeitslehre</t>
   </si>
   <si>
     <t>Statistik</t>
@@ -1014,6 +1049,15 @@
     <t>Strömungsmechanik</t>
   </si>
   <si>
+    <t>Studienarbeit (Angewandte Informatik)</t>
+  </si>
+  <si>
+    <t>Studienarbeit Elektrotechnik</t>
+  </si>
+  <si>
+    <t>Studienarbeit (Projekt 2) Ingenieurinformatik</t>
+  </si>
+  <si>
     <t>Supply Chain Management</t>
   </si>
   <si>
@@ -1065,7 +1109,7 @@
     <t>Thermodynamik</t>
   </si>
   <si>
-    <t>Transport,- Speditions-, Zoll- und Außenhandelsrecht</t>
+    <t>Transport- Speditions- Zoll- und Außenhandelsrecht</t>
   </si>
   <si>
     <t>Transportlogistik</t>
@@ -1146,20 +1190,317 @@
     <t>Zukunfttechnologien und Nachhaltigkeit</t>
   </si>
   <si>
-    <t>Zulassung und Recht, formelle Randbedingungen Eisenbahnbetrieb</t>
+    <t>Zulassung und Recht formelle Randbedingungen Eisenbahnbetrieb</t>
   </si>
   <si>
     <t>Zustandsbeobachtung und -schätzung</t>
   </si>
   <si>
     <t>Zustandsregelungen</t>
+  </si>
+  <si>
+    <t>Bachelorstudiengang</t>
+  </si>
+  <si>
+    <t>Studienart</t>
+  </si>
+  <si>
+    <t>Vertiefung</t>
+  </si>
+  <si>
+    <t>Pflichtmodule</t>
+  </si>
+  <si>
+    <t>Wahlpflichtmodule</t>
+  </si>
+  <si>
+    <t>praxisintegriert</t>
+  </si>
+  <si>
+    <t>Logistik</t>
+  </si>
+  <si>
+    <t>Grundlagen der Programmierung, Grundlagen der Wirtschaftswissenschaften, Mathematik 1, Physik, Zukunfstechnologien und Nachhaltigkeit, Beschaffung Produktion und Logistik, Datenbanken, Externes Rechnungswesen und Finanzierung, Mathematik 2, Technische Mechanik - Statik und Festigkeitslehre, Geschäftsprozessmodellierung und IT - Systeme, Statistik, Technisches Englisch, Lean Production &amp; Industrial Engineering, Marketing und technischer Vertrieb, Materialflusssysteme, Operations Research, Digitale Fabrikplanung und Simulation, Fördertechnik, Internes Rechnungswesen, und Investition, Produktionsplanung und Steuerung, Transportlogistik, Cyberphysische Logistiksysteme, Industrielles Datenmanagement, Planung und Controlling, Supply Chain Management, Personal und Organisation, Qualitätsmanagement</t>
+  </si>
+  <si>
+    <t>Grundlagen der Programmierung, Grundlagen der Wirtschaftswissenschaften, Mathematik 1, Physik, Zukunfstechnologien und Nachhaltigkeit, Beschaffung Produktion und Logistik, Datenbanken, Externes Rechnungswesen und Finanzierung, Mathematik 2, Technische Mechanik - Statik und Festigkeitslehre, Geschäftsprozessmodellierung und IT - Systeme, Statistik, Technisches Englisch, Grundlagen der Elektrischen Messtechnik, Grundlagen der Konstruktion, Lean Production &amp; Industrial Engineering, Marketing und technischer Vertrieb, Internes Rechnungswesen und Investition, Regelungstechnik, Werkstofftechnik, Wahlmodul, Wahlmodul, Industrielle Steuerungstechnik, Planung und Controlling, Wahlmodul, Wahlmodul, Personal und Organisation, Qualitätsmanagement</t>
+  </si>
+  <si>
+    <t>Changemanagement, Digitale Fabrikplanung und Simulation, Digitaltechnik, E-Business &amp; Online Marketing, Elektrische Maschinen, Fertigungstechnik, Halbleiterbauelemente und Schaltungen, Industrielle Kommunikation, Leistungselektronik, Materialflusssysteme, Mechatronische Systeme 1, Messtechnik und Sensorik, Methodisches Konstruieren und CAD, Mikrocontrollerprogrammierung, Strategisches Marketing</t>
+  </si>
+  <si>
+    <t>Vollzeit</t>
+  </si>
+  <si>
+    <t>Mobilität</t>
+  </si>
+  <si>
+    <t>Allgemeine Betriebswirtschaftslehre, Allgemeine Volkswirtschaftslehre, Berufsfeldorientiertes Arbeiten, Mathematik 1, Physik, Technische Mechanik, Grundlagen der Elektrotechnik, Internes Rechnungswesen, Konstruktion, Marketing, Mathematik 2, Werkstofftechnik, Anwendungen und Methoden der Elektrotechnik, Einführung in die Informatik, Externes Rechnungswesen, Innovations- und Projektmanagement, Investition und Finanzierung, Maschinenelemente, Angewandte Informatik, Controlling, Grundlagen Produktion und Logistik, Mess- und Systemtechnik, Produktionstechnik, Statistik, English for Business and Engineering 1, Fahrzeugdynamik, Projekt, Regelungs- und Automatisierungssysteme, Schienenfahrzeugtechnik, Wahmodul, Fahrerassistenzsysteme und automatisiertes Fahren, Personal und Organisation, Projekt Mobilität, Qualitätsmanagement, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Einführung System Bahn, Electromobility, Elektrische Antriebssysteme, Mikromobilität, Optische Systeme in mobilen und autonomen Anwendungen, Sensor- und Aktorsysteme, Verkehrswirtschaft, Betriebswirtschaftliche Steuerlehre, Digitale Transformation von industriellen Unternehmensprozessen, English for Business und Engineering 2, Gender und Diversity: Erfolgsfaktoren für Unternehmen, International Activities, Textile Technologies</t>
+  </si>
+  <si>
+    <t>Nachhaltige Produkte und Prozesse</t>
+  </si>
+  <si>
+    <t>Allgemeine Betriebswirtschaftslehre, Allgemeine Volkswirtschaftslehre, Berufsfeldorientiertes Arbeiten, Mathematik 1, Physik, Technische Mechanik, Grundlagen der Elektrotechnik, Internes Rechnungswesen, Konstruktion, Marketing, Mathematik 2, Werkstofftechnik, Anwendungen und Methoden der Elektrotechnik, Einführung in die Informatik, Externes Rechnungswesen, Innovations- und Projektmanagement, Investition und Finanzierung, Maschinenelemente, Angewandte Informatik, Controlling, Grundlagen Produktion und Logistik, Mess- und Systemtechnik, Produktionstechnik, Statistik, English for Business and Engineering 1, Regelungs- und Automatisierungssysteme, Wahlmodul, Wahlmodul, Zirkuläre Wertschöpfung, Nachhaltigkeitsbewertung und -analyse, Personal und Organisation, Qualitätsmanagement, Wahlmodul, Wahlmodul, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Digitale Transformation von industriellen Unternehmensprozessen, Electromobility, Energiemanagement, Integrierte Produktentwicklung, Nachhaltige Gebäude, Photovoltaik, Produk-Risikomanagement, Projekt Nachhaltige Produkte und Prozesse, Sensorik, Thermische Nutzung regenerativer Energien, Wind- und Wasserkraft, Betriebswirtschaftliche Steuerlehre, Digitale Transformation von industriellen Unternehmensprozessen, English for Business und Engineering 2, Gender und Diversity: Erfolgsfaktoren für Unternehmen, International Activities, Textile Technologies</t>
+  </si>
+  <si>
+    <t>Produktion und Logistik</t>
+  </si>
+  <si>
+    <t>Allgemeine Betriebswirtschaftslehre, Allgemeine Volkswirtschaftslehre, Berufsfeldorientiertes Arbeiten, Mathematik 1, Physik, Technische Mechanik, Grundlagen der Elektrotechnik, Internes Rechnungswesen, Konstruktion, Marketing, Mathematik 2, Werkstofftechnik, Anwendungen und Methoden der Elektrotechnik, Einführung in die Informatik, Externes Rechnungswesen, Innovations- und Projektmanagement, Investition und Finanzierung, Maschinenelemente, Angewandte Informatik, Controlling, Grundlagen Produktion und Logistik, Mess- und Systemtechnik, Produktionstechnik, Statistik, English for Business and Engineering 1, Regelungs- und Automatisierungssysteme, Wahlmodul, Wahlmodul, Wahlmodul, Personal und Organisation, Qualitätsmanagement, Wahlmodul, Wahlmodul, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Angewandte Produktion, Digitale Fabrikplanung und Simulation, Digitale Transformation von industriellen Unternehmensprozessen, Diskrete Mathematik, Fabrikplanung, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Lean Production, Operations Research, Produktionsautomatisierung und -digitalisierung, Produktionsplanung und -steuerung, Projekt Produktion und Logistik, Robotik - Einführung und Grundlagen, Spieltheorie, Supply Chain Management, Werkzeugmaschinen, Betriebswirtschaftliche Steuerlehre, Digitale Transformation von industriellen Unternehmensprozessen, English for Business und Engineering 2, Gender und Diversity: Erfolgsfaktoren für Unternehmen, International Activities, Textile Technologies</t>
+  </si>
+  <si>
+    <t>Technischer Vertrieb</t>
+  </si>
+  <si>
+    <t>Beschaffungsmanagement, Betriebswirtschaftliche Unternehmensführung, Digitale Transformation von industriellen Unternehmensprozessen, Electronic Marketing, Industriegütermarketing, Internationales Marketing, Marktforschung, Produkt- und Dienstleistungsmanagement, Produkt-Risikomanagement, Projekt Technischer Vertrieb, Vertriebsmanagement, Betriebswirtschaftliche Steuerlehre, Digitale Transformation von industriellen Unternehmensprozessen, English for Business und Engineering 2, Gender und Diversity: Erfolgsfaktoren für Unternehmen, International Activities, Textile Technologies</t>
+  </si>
+  <si>
+    <t>Einführung in das Berufsfeld Software Engineering, Grundlagen der Betriebswirtschaftslehre, Grundlagen der Informatik, Mathematik 1, Rechner- und Betriebssysteme, Algorithmen und Datenstrukturen, Datenbanken, Mathematik 2, Objektorientierte Programmierung, Statistik, HMI und Bedienoberflächen, Mikrocontrollerprogrammierung, Technisches Englisch, Vernetzung und IoT-Lösungen, Wahlmodul, Data Analytics, IT-Security, Wahlmodul, Web-Technologien, Innovations- und Projektmanagement, Software Engineering, xReality Technologien, Wahlmodul, Wahlmodul, E-Business &amp; Online Marketing, IT-Product Engineering, Wahlmodul, Wahlmodul, Business Intelligence, Industrielle Anwendungssysteme</t>
+  </si>
+  <si>
+    <t>Big Data, Change Management, Data Mining, Grundlagen der Elektrischen Messtechnik, Industrielle Kommunikation, Maschinelles Lernen, Produktentwicklung und Requirement Engineering, Web-Technologien 2, Geschäftsprozessmodellierung und IT-Systeme, Grundlagen der Elektrotechnik, Operations Research, Industrielle Steuerungstechnik</t>
+  </si>
+  <si>
+    <t>Regenerative Energien</t>
+  </si>
+  <si>
+    <t>Energie und Effizienz</t>
+  </si>
+  <si>
+    <t>Chemie, Elektrotechnik 1, Ingenieurmathematik 1, Physik 1, Regenerative Energiewirtschaft, Biochemie und Mikrobiologie, Elektronik, Elektrotechnik 2, Ingenieurmathematik 2, Messtechnik, Physik 2, Allgemeine Betriebswirtschaftslehre, Automatisierungstechnik, Grundlagen der Informatik, Grundlagen der elektrischen Energietechnik, Technisches Englisch 1, Verfahrenstechnik, Anwendungen der Informatik, Elektrische Energiespeicher und Brennstoffzellen, Leistungselektronik, Regelungstechnik, Wind- und Wasserkraft, Dezentrale Energiesysteme, Effiziente Lichttechnik, Energiemanagement, Projekt Energie und Effizienz, Wahlmodul, Wahlmodul, Anlagenplanung, Energiepolitik und -wirtschaft, Photovoltaik, Thermische Nutzung regenerativer Energien, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Antriebstechnik, Biogas und Bioraffinerien, Elektrische Maschinen, Elektrische Netze, Elektrotechnik 3, Feldsimulation, Gender und Diversity: Erfolgsfaktoren für Unternehmen, International Activities, Investition und Finanzierung, Signale und Systeme, Technisches Englisch 2, Textile Technologies, Zustandsregelungen, Electromobility, Elektrische Maschinen, Hochspannungstechnik, Modellbildung und Simulation, Nachhaltige Gebäude, Sensorik, Thermodynamik, Vernetzte Systeme mit Mikrocontrollern, Wasserstoff in der Energieversorgung</t>
+  </si>
+  <si>
+    <t>Chemie, Elektrotechnik 1, Ingenieurmathematik 1, Physik 1, Regenerative Energiewirtschaft, Biochemie und Mikrobiologie, Elektronik, Elektrotechnik 2, Ingenieurmathematik 2, Messtechnik, Physik 2, Allgemeine Betriebswirtschaftslehre, Automatisierungstechnik, Grundlagen der Informatik, Grundlagen der elektrischen Energietechnik, Technisches Englisch 1, Verfahrenstechnik, Anwendungen der Informatik, Elektrische Energiespeicher und Brennstoffzellen, Leistungselektronik, Regelungstechnik, Wind- und Wasserkraft, Dezentrale Energiesysteme, Effiziente Lichttechnik, Projekt Nachhaltige Produkte und Prozesse, Wahlmodul, Wahlmodul, Zirkuläre Wertschöpfung, Anlagenplanung, Nachhaltigkeitsbewertung und -analyse, Photovoltaik, Produktion-Risikomanagement, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Antriebstechnik, Biogas und Bioraffinerien, Elektrische Maschinen, Elektrische Netze, Elektrotechnik 3, Feldsimulation, Gender und Diversity: Erfolgsfaktoren für Unternehmen, International Activities, Investition und Finanzierung, Signale und Systeme, Technisches Englisch 2, Textile Technologies, Zustandsregelungen, Electromobility, Energiemanagement, Innovations- und Projektmanagement, Integrierte Produktentwicklung, Nachhaltige Gebäude, Sensorik, Thermische Nutzung regenerativer Energien, Werkstofftechnik</t>
+  </si>
+  <si>
+    <t>Product Service Engineering</t>
+  </si>
+  <si>
+    <t>Elektrotechnik 1, Grundlagen der Betriebswirtschaftslehre, Grundlagen der Informatik, Mathematik 1, Product-Service Engineering - Einführung und Übersicht, Datenbanken, Elektrotechnik 2, Grundlagen der Mechanik, Mathematik 2, Objektorientierte Programmierung, HMI und Bedienoberflächen, Kostenrechnung/Produktkalkulation, Mathematik 3, Messtechnik / Sensorik, Technisches Englisch, Grundlagen der Konstruktion, Industrielle Steuerungstechnik, Regelungstechnik, Service Engineering, Statistik, Innovations- und Projektmanagement, Vernetzung und IoT-Lösungen, Wahlmodul, Wahlmodul, Produktentwicklung und Requirement Engineering, Safety und Security, Wahlmodul, Wahlmodul, Diagnose und Predictive Maintenance, Vertriebs- und Kundenmanagement</t>
+  </si>
+  <si>
+    <t>Data Analytics, Instandhaltungs- und Ersatzteilmanagement, Maschinelles Lernen, Qualitätsmanagement, Servicekommunikation/ Trainingskonzeption, Smart Services und -Devices, Usability Engineering, Vertrags- und Haftungsrecht</t>
+  </si>
+  <si>
+    <t>Mechatronik</t>
+  </si>
+  <si>
+    <t>Autonome Systeme und Robotik</t>
+  </si>
+  <si>
+    <t>Einführung in die Mechatronik, Elektrotechnik 1 - Gleichstromlehre, Informatik 1 - Imperative Programmierung, Konstruktion, Mathematik 1, Technische Mechanik 1, Elektrotechnik 2 - Wechselstromlehre, Informatik 2 - Objektorientierte Programmierung, Mathematik 2, Physikalische und messtechnische Grundlagen, Technische Mechanik 2, Werkstofftechnik, Grundlagen der Analog-und Digitalelektronik, Innovations- und Projektmanagement, Maschinenelemente, Mathematik 3, Regelungstechnik, Robotik - Einführung und Grundlagen, Eingebettete Systeme in der Mechatronik, Elektrische Antriebssysteme, Finite Elemente Methode, Sensor- und Aktorsysteme, Technisches Englisch, Verteilte Systeme, Maschinelles Lernen, Modellbildung und Simulation, Programmierung autonomer Roboter, Projekt Mechatronik, Wahlmodul, Wahlmodul, Allgemeine Betriebswirtschaftslehre, Cooperative and Wearable Robotics, Projekt Autonome Systeme und Robotik, Wahlmodul, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Akustische Signalverarbeitung in technischen und biologischen Systemen, Elektrotechnik 3, Feldsimulation, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Grundlagen Data Science, Integrierte Produktentwicklung, International Activities, Mess- und Prüfsysteme, Motion Control, Optische Technologien, Produktionstechnik, Projekt Mechatronik, Qualitätsmanagement, Rechnerarchitekturen, Signale und Systeme, Textile Technologies, Bildverarbeitung und Mustererkennung, Optische Systemtechnik, Photovoltaik, Software Engineering, Vernetzte Systeme mit Mikrocontrollern</t>
+  </si>
+  <si>
+    <t>Berufliche Bildung</t>
+  </si>
+  <si>
+    <t>Akustische Signalverarbeitung in technischen und biologischen Systemen, Elektrotechnik 3, Feldsimulation, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Grundlagen Data Science, Integrierte Produktentwicklung, International Activities, Mess- und Prüfsysteme, Motion Control, Optische Technologien, Produktionstechnik, Projekt Mechatronik, Qualitätsmanagement, Rechnerarchitekturen, Signale und Systeme, Textile Technologies</t>
+  </si>
+  <si>
+    <t>Medizintechnik</t>
+  </si>
+  <si>
+    <t>Akustische Signalverarbeitung in technischen und biologischen Systemen, Elektrotechnik 3, Feldsimulation, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Grundlagen Data Science, Integrierte Produktentwicklung, International Activities, Mess- und Prüfsysteme, Motion Control, Optische Technologien, Produktionstechnik, Projekt Mechatronik, Qualitätsmanagement, Rechnerarchitekturen, Signale und Systeme, Textile Technologies, Aktuelle Themen der Medizintechnik, Biosignalverarbeitung und Neuroengineering, Biotechnologische Detektionssysteme, Biotechnologische Produktionsprozesse, Cooperative and Wearable Robotics, KI-basierte Medizinische Bildverarbeitung, Medizinische Bildgebungsverfahren, Medizinische Datenverarbeitung, Neuroanatomie/-physiologie und Neurorehabilitation, Projekt Medizintechnik</t>
+  </si>
+  <si>
+    <t>Akustische Signalverarbeitung in technischen und biologischen Systemen, Elektrotechnik 3, Feldsimulation, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Grundlagen Data Science, Integrierte Produktentwicklung, International Activities, Mess- und Prüfsysteme, Motion Control, Optische Technologien, Produktionstechnik, Projekt Mechatronik, Qualitätsmanagement, Rechnerarchitekturen, Signale und Systeme, Textile Technologies, Einführung System Bahn, Electromobility, Mikromobilität, Optische Systeme in mobilen und autonomen Anwendungen, Sensorik, Verkehrswirtschaft</t>
+  </si>
+  <si>
+    <t>Akustische Signalverarbeitung in technischen und biologischen Systemen, Elektrotechnik 3, Feldsimulation, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Grundlagen Data Science, Integrierte Produktentwicklung, International Activities, Mess- und Prüfsysteme, Motion Control, Optische Technologien, Produktionstechnik, Projekt Mechatronik, Qualitätsmanagement, Rechnerarchitekturen, Signale und Systeme, Textile Technologies, Electromobility, Energiemanagement, Nachhaltige Gebäude, Photovoltaik, Produkt-Risikomanagement, Sensorik, Thermische Nutzung regenerativer Energien, Wind- und Wasserkraft</t>
+  </si>
+  <si>
+    <t>Datenbanken, Grundlagen der Elektrotechnik, Informatik 1, Mathematik A, Technisches Englisch 1, Algorithmen und Datenstrukturen, Betriebssysteme, Informatik 2, Mathematik B, Mathematik C, Physik für Informatiker, Automatisierungstechnik, Digitalelektronik, Komplexe Robotische Bewegungssysteme, Netzwerktechnik, Numerische Mathematik, Software Engineering, Bildverarbeitung und Mustererkennung, Mikrocontroller, Numerische Simulation, Rechnerarchitekturen, Regelungstechnik, Wahlmodul, Allgemeine Betriebswirtschaftslehre, Wahlmodul, High Performance Computing, IT-Sicherheit, Verteilte Software-Anwendungen, Studienarbeit (Angewandte Informatik), Wahlmodul, Wahlmodul, Wahlmodul, Wahlmodul, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aktuelle Themen der Medizintechnik, Ambient Assisted Living, Auslandsaufenthalt, Cooperative and Wearable Robotics, Electronic Marketing, Elektrotechnik 3, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Grundlagen Data Science, Grundlagen der Kryptographie, Integrierte Produktentwicklung, International Activities, Internationales Marketing, Internes Rechnungswesen, Investition und Finanzierung, KI-basierte Medizinische Bildverarbeitung, Künstliche Neuronale Netze, Maschinelles Lernen, Medizinische Bildgebungsverfahren, Medizinische Datenverarbeitung, Messtechnik, Mikrosystemtechnik, Motion Control, Natural Language Processing, Optoelektronik, Personal und Organisation, Qualitätsmanagement, Robotik - Einführung und Grundlagen, Sensor- und Aktorsysteme, Sensorik, Signale und Systeme, Stochastik, Technisches Englisch 2, Theoretische Informatik, Vernetzte Systeme mit Mikrocontrollern, Web-Technologien 1, Web-Technologien 2, Biotechnologische Detektionssysteme, Biotechnologische Produktionsprozesse, Mess- und Prüfsysteme, Modellbildung und Simulation, Motion Control, Predictive Analytics, Projekt Automatisierungstechnik, Sensor- und Aktorsysteme, Vernetzte Systeme mit Mikrocontrollern, Zustandsbeobachtung und -schätzung, Zustandsregelungen
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aktuelle Themen der Medizintechnik, Ambient Assisted Living, Auslandsaufenthalt, Cooperative and Wearable Robotics, Electronic Marketing, Elektrotechnik 3, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Grundlagen Data Science, Grundlagen der Kryptographie, Integrierte Produktentwicklung, International Activities, Internationales Marketing, Internes Rechnungswesen, Investition und Finanzierung, KI-basierte Medizinische Bildverarbeitung, Künstliche Neuronale Netze, Maschinelles Lernen, Medizinische Bildgebungsverfahren, Medizinische Datenverarbeitung, Messtechnik, Mikrosystemtechnik, Motion Control, Natural Language Processing, Optoelektronik, Personal und Organisation, Qualitätsmanagement, Robotik - Einführung und Grundlagen, Sensor- und Aktorsysteme, Sensorik, Signale und Systeme, Stochastik, Technisches Englisch 2, Theoretische Informatik, Vernetzte Systeme mit Mikrocontrollern, Web-Technologien 1, Web-Technologien 2, Antriebstechnik, Elektrische Antriebssysteme, Konstruktion, Motion Control, Optische Systemtechnik, Photovoltaik, Programmierung autonomer Roboter, Sensor- und Aktorsysteme, Vernetzte Systeme mit Mikrocontrollern
+</t>
+  </si>
+  <si>
+    <t>Aktuelle Themen der Medizintechnik, Ambient Assisted Living, Auslandsaufenthalt, Cooperative and Wearable Robotics, Electronic Marketing, Elektrotechnik 3, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Grundlagen Data Science, Grundlagen der Kryptographie, Integrierte Produktentwicklung, International Activities, Internationales Marketing, Internes Rechnungswesen, Investition und Finanzierung, KI-basierte Medizinische Bildverarbeitung, Künstliche Neuronale Netze, Maschinelles Lernen, Medizinische Bildgebungsverfahren, Medizinische Datenverarbeitung, Messtechnik, Mikrosystemtechnik, Motion Control, Natural Language Processing, Optoelektronik, Personal und Organisation, Qualitätsmanagement, Robotik - Einführung und Grundlagen, Sensor- und Aktorsysteme, Sensorik, Signale und Systeme, Stochastik, Technisches Englisch 2, Theoretische Informatik, Vernetzte Systeme mit Mikrocontrollern, Web-Technologien 1, Web-Technologien 2, Aktuelle Themen der Medizintechnik, Akustische Signalverarbeitung in technischen und biologischen Systemen, Biosignalverarbeitung und Neuroengineering, Biotechnologische Detektionssysteme, Biotechnologische Produktionsprozesse, Cooperative and Wearable Robotics, KI-basierte Medizinische Bildverarbeitung, Medizinische Bildgebungsverfahren, Medizinische Datenverarbeitung, Neuroanatomie/-physiologie und Neurorehabilitation, Projekt Medizintechnik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aktuelle Themen der Medizintechnik, Ambient Assisted Living, Auslandsaufenthalt, Cooperative and Wearable Robotics, Electronic Marketing, Elektrotechnik 3, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Grundlagen Data Science, Grundlagen der Kryptographie, Integrierte Produktentwicklung, International Activities, Internationales Marketing, Internes Rechnungswesen, Investition und Finanzierung, KI-basierte Medizinische Bildverarbeitung, Künstliche Neuronale Netze, Maschinelles Lernen, Medizinische Bildgebungsverfahren, Medizinische Datenverarbeitung, Messtechnik, Mikrosystemtechnik, Motion Control, Natural Language Processing, Optoelektronik, Personal und Organisation, Qualitätsmanagement, Robotik - Einführung und Grundlagen, Sensor- und Aktorsysteme, Sensorik, Signale und Systeme, Stochastik, Technisches Englisch 2, Theoretische Informatik, Vernetzte Systeme mit Mikrocontrollern, Web-Technologien 1, Web-Technologien 2, Diskrete Mathematik, Grundlagen der Kryptographie, Predictive Analytics, Stochastik
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elektotechnik </t>
+  </si>
+  <si>
+    <t>Elektrotechnik 1, Informatik 1, Ingenieurmathematik 1, Physik 1, Werkstoffe der Elektrotechnik und
+Elektronik, Elektronische Bauelemente, Elektrotechnik 2, Informatik 2, Ingenieurmathematik 2, Messtechnik, Physik 2, Analoge und digitale Schaltungstechnik, Automatisierungstechnik, Elektrische Maschinen, Elektrotechnik 3, Grundlagen der elektrischen Energietechnik, Sensorik, Elektromagnetische Verträglichkeit, Leistungselektronik, Mikrosystemetechnik, Numerik für ET-Ingenieure, Reglungstechnik, Signale und Systeme, Elektrische Energieerzeugung und -verteilung 1, Optoelektronik, Technisches Englisch 1, Energiemanagement, Projekt Energie und Effizienz, Wahlmodul, Allgemeine Betriebswirtschaftslehre, Studienarbeit Elektrotechnik Elektrotechnik, Energiepolitik und -wirtschaft, Thermische Nutzung regenerativer Energien, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Anlagenplanung, Dezentrale Energiesysteme, Effiziente Lichttechnik, Electromobility, Elektrische Energiespeicher und Brennstoffzellen, Hochspannungstechnik, Modelbildung und Simulation, Nachhaltige Gebäude, Photovoltaik, Thermodynamik, Vernetzte Systeme mit Mikrocontrollern, Wasserstoff in der Energieversorgung, Wind- und Wasserkraft</t>
+  </si>
+  <si>
+    <t>Elektrotechnik 1, Informatik 1, Ingenieurmathematik 1, Physik 1, Werkstoffe der Elektrotechnik und
+Elektronik, Elektronische Bauelemente, Elektrotechnik 2, Informatik 2, Ingenieurmathematik 2, Messtechnik, Physik 2, Analoge und digitale Schaltungstechnik, Automatisierungstechnik, Elektrische Maschinen, Elektrotechnik 3, Grundlagen der elektrischen Energietechnik, Sensorik, Elektromagnetische Verträglichkeit, Leistungselektronik, Mikrosystemetechnik, Numerik für ET-Ingenieure, Reglungstechnik, Signale und Systeme, Elektrische Energieerzeugung und -verteilung 1, Optoelektronik, Technisches Englisch 1, Wahlmodul, Wahlmodul, Wahlmodul, Allgemeine Betriebswirtschaftslehre, Studienarbeit Elektrotechnik, Wahlmodul, Wahlmodul, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Aktuelle Themen der Medizintechnik, Akustische Signalverarbeitung in technischen und biologischen Systemen, Biosignalverarbeitung und Neuroengineering, Biotechnologische Detektionssysteme, Biotechnologische Produktionsprozesse, Cooperative and Wearable Robotics, KI-basierte Medizinische Bildverarbeitung, Medizinische Bildgebungsverfahren, Medizinische Datenverarbeitung, Neuroanatomie/-physiologie und Neurorehabilitation, Projekt Medizintechnik, Antriebstechnik, Auslandsaufenthalt, Embedded Systems, Feldsimulation, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Hochspannungstechnik, International Activities, Mikrocontroller</t>
+  </si>
+  <si>
+    <t>Antriebstechnik, Auslandsaufenthalt, Embedded Systems, Feldsimulation, Gender und Diversity: Erfolgsfaktoren
+für Unternehmen, Hochspannungstechnik, International Activities, Mikrocontroller</t>
+  </si>
+  <si>
+    <t>Elektrotechnik 1, Informatik 1, Ingenieurmathematik 1, Physik 1, Werkstoffe der Elektrotechnik und
+Elektronik, Elektronische Bauelemente, Elektrotechnik 2, Informatik 2, Ingenieurmathematik 2, Messtechnik, Physik 2, Analoge und digitale Schaltungstechnik, Automatisierungstechnik, Elektrische Maschinen, Elektrotechnik 3, Grundlagen der elektrischen Energietechnik, Sensorik, Elektromagnetische Verträglichkeit, Leistungselektronik, Mikrosystemetechnik, Numerik für ET-Ingenieure, Reglungstechnik, Signale und Systeme, Elektrische Energieerzeugung und -verteilung 1, Optoelektronik, Technisches Englisch 1, Allgemeine Didaktik mit Eignungs- und
+Orientierungspraktikum, Berufspädagogik 1 und Berufsfeldpraktikum, Diagnose und Förderung, Allgemeine Betriebswirtschaftslehre, Studienarbeit Elektrotechnik, Berufspädagogik 2, Projekt Berufliche Bildung, Technikdidaktik, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Elektrotechnik 1, Informatik 1, Ingenieurmathematik 1, Physik 1, Werkstoffe der Elektrotechnik und
+Elektronik, Elektronische Bauelemente, Elektrotechnik 2, Informatik 2, Ingenieurmathematik 2, Messtechnik, Physik 2, Analoge und digitale Schaltungstechnik, Automatisierungstechnik, Elektrische Maschinen, Elektrotechnik 3, Grundlagen der elektrischen Energietechnik, Sensorik, Elektromagnetische Verträglichkeit, Leistungselektronik, Mikrosystemetechnik, Numerik für ET-Ingenieure, Reglungstechnik, Signale und Systeme, Elektrische Energieerzeugung und -verteilung 1, Optoelektronik, Technisches Englisch 1, Fahrzeugdynamik, Schienenfahrzeugtechnik, Wahlmodul, Allgemeine Betriebswirtschaftslehre, Studienarbeit Elektrotechnik, Projekt Mobilität, Fahrerassistenzsysteme und automatisiertes Fahren, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Einführung System Bahn, Electromobility, Mikromobilität, Gender und Diversity: Erfolgsfaktoren
+für Unternehmen, Optische Systeme in mobilen und autonomen Anwendungen, Sensor- und Aktorsysteme, Verkehrswirtschaft, Antriebstechnik, Auslandsaufenthalt, Embedded Systems, Feldsimulation, Hochspannungstechnik, International Activities, Mikrocontroller</t>
+  </si>
+  <si>
+    <t>Energie- und Automatisierungstechnik</t>
+  </si>
+  <si>
+    <t>Grundlagen der Elektrotechnik 1, Mathematik 1, Physik 1, Werkstoffe der Elektrotechnik, Grundlagen der Elektrotechnik 2, Mathematik 2, Physik 2, Technisches Englisch, Elektronik, Grundlagen der Energietechnik, Mathematik 3, Messtechnik, Elektrische Maschinen, Grundzüge der BWL für Ingenieure, Informatik, Mathematik 4, Angewandte Informatik, Effiziente Lichttechnik, Elektrische Netze, Reglungstechnik, Automatisierungssysteme, Energiesysteme, Ingenieurwissenschaftliches Projekt, Leistungselektronik, Antriebstechnik, Produkt- und Risikomanagement, Erneuerbare und konventionelle Energieerzeugung, Qualitätsmanagement, Berufspädagogik 1 und Berufsfeldpraktikum, Diagnose und Förderung, Berufspädagogik 2, Technikdidaktik</t>
+  </si>
+  <si>
+    <t>Weiterbildung</t>
+  </si>
+  <si>
+    <t>Grundlagen der Elektrotechnik 1, Mathematik 1, Physik 1, Werkstoffe der Elektrotechnik, Grundlagen der Elektrotechnik 2, Mathematik 2, Physik 2, Technisches Englisch, Elektronik, Grundlagen der Energietechnik, Mathematik 3, Messtechnik, Elektrische Maschinen, Grundzüge der BWL für Ingenieure, Informatik, Mathematik 4, Angewandte Informatik, Effiziente Lichttechnik, Elektrische Netze, Reglungstechnik, Automatisierungssysteme, Energiesysteme, Ingenieurwissenschaftliches Projekt, Leistungselektronik, Antriebstechnik, Produkt- und Risikomanagement, Erneuerbare und konventionelle Energieerzeugung, Qualitätsmanagement, Mechatronische Systeme, Moderne Energiepolitik, Data Science, Hochspannungstechnik</t>
+  </si>
+  <si>
+    <t>Ingenieurinformatik</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Einführung in die Ingenieurinformatik, Informatik 1, Mathematik A, Physik 1, Technisches Englisch 1, Algorithmen und Datenstrukturen, Elektrotechnische Grundlagen, Informatik 2, Mathematik B, Mathematik C, Physik 2, Automatisierungstechnik, Betriebswirtschaftslehre, Digitalelektronik 1, Netzwerktechnik, Software Engineering, Teamprojekt Ingenieurinformatik, Bildverarbeitung und Mustererkennung, Digitalelektronik 2, Maschinelles Lernen und Data Mining, Numerische Mathematik, Reglungstechnik, Wahlmodul, Mikrocontroller, Numerische Simulation, Rechnerarchitekturen, Simulationstechnik,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> Studienarbeit (Projekt 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>) Ingenieurinformatik, Wahlmodul, Betriebssysteme, Datenbank-Anwendungen, Embedded Systems, High Performance Computing, Wahlmodul, Wahlmodul</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ambient Assisted Living, Assistenzsysteme, Cluster Computing, Data Mining, Gebäudeautomation, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Geschäftsprozessmodellierung und IT-Systeme, Hochfrequenzelektronik, IT-Sicherheitsmanagement, Innovations- und Projektmanagement, Integrierte Produktentwicklung, Intelligente Sensorsysteme, Internationales Management/ Marketing, Investition und Finanzierung, Kosten- und Leistungsrechnung, Kryptographie, Leistungselektronik, Marketing und technischer Vertrieb, Messtechnik, Mikrosystemtechnik, Netzwerke und Bussysteme, Optische Systemtechnik, Optoelektronik, Personal und Organisation, Qualitätsmanagement, Robotik, Sensorik, Signale und Systeme, Social Media und Natural Language Processing, Statistik, Technisches Englsich 2, Theoretische Informatik </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maschinenbau </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einführung Maschinenbau, Festigkeitslehre, Mathematik 1, Statik, Technisches Zeichnen, Werkstofftechnik, Dynamik, Kunststofftechnik, Mathematik 2, Physik, Thermodynamik, Verbindungselemente, Basisprojekt, Getriebeelemente, Mathematik 3, Produktionstechnik, Prozess- und Informationsmanagement, Elektrische Maschinen, Strömungsmechanik, System- und Messtechnik, Technisches Englisch, Steuerungs- und Regelungstechnik, Vertiefungsprojekt, Allgemeine Betriebswirtschaftslehre, Qualitätsmanagement, Wahlmodul, Werkzeugmaschinen, Produktionsautomatisierung und digitalisierung, Fabrikplanung, Angewandte Produktion, Innovations- und Projektmanagement, Lean Production, Grundlagen Produktion und Logistik, Wahlmodul, Wahlmodul </t>
+  </si>
+  <si>
+    <t>Allgemeine Didaktik mit Eignungs- und Orientierungspraktikum, Auslandsaufenthalt, Berufspädagogik 1 und Berufsfeldpraktikum, Berufspädagogik 2, Diagnose und Förderung, Gender und Diversity: Erfolgsfaktoren
+für Unternehmen, International Activities , Technikdidaktik, CAD, Digitale Fabrikplanung und Simulation, Kunststoffverarbeitung, Leichtbauwerkstoffe, Operations Research, Personal und Organisation, Produktionsplanung und -steuerung, Robotik - Einführung und Grundlagen, Spieltheorie, Supply Chain Management, Unternehmensplanspiel Logistik oder General Management</t>
+  </si>
+  <si>
+    <t>Energietechnik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einführung Maschinenbau, Festigkeitslehre, Mathematik 1, Statik, Technisches Zeichnen, Werkstofftechnik, Dynamik, Kunststofftechnik, Mathematik 2, Physik, Thermodynamik, Verbindungselemente, Basisprojekt, Getriebeelemente, Mathematik 3, Produktionstechnik, Prozess- und Informationsmanagement, Elektrische Maschinen, Strömungsmechanik, System- und Messtechnik, Technisches Englisch, Steuerungs- und Regelungstechnik, Vertiefungsprojekt, Allgemeine Betriebswirtschaftslehre, Qualitätsmanagement, Wahlmodul, Wahlmodul, Wärmeübertragung und Wärmespeicher, Thermodynamik der Energietechnik, Wahlmodul, Energieeffiziente Heiz- und Kühlsysteme im Anlagenbau, Energietechnik und Wasserstofftechnologie </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allgemeine Didaktik mit Eignungs- und Orientierungspraktikum, Auslandsaufenthalt, Berufspädagogik 1 und Berufsfeldpraktikum, Berufspädagogik 2, Diagnose und Förderung, Gender und Diversity: Erfolgsfaktoren
+für Unternehmen, International Activities , Technikdidaktik, CAD, Elektrische Energiespeicher und
+Brennstoffzellen, Energiemanagement, Maschinendynamik, Numerische Strömungstechnik 1, Photovoltaik, Thermische Nutzung regenerativer Energien, Werkstoff- und Bauteilprüfung, Wind- und Wasserkraft </t>
+  </si>
+  <si>
+    <t>Konstruktion und Entwicklung</t>
+  </si>
+  <si>
+    <t>Einführung Maschinenbau, Festigkeitslehre, Mathematik 1, Statik, Technisches Zeichnen, Werkstofftechnik, Dynamik, Kunststofftechnik, Mathematik 2, Physik, Thermodynamik, Verbindungselemente, Basisprojekt, Getriebeelemente, Mathematik 3, Produktionstechnik, Prozess- und Informationsmanagement, Elektrische Maschinen, Strömungsmechanik, System- und Messtechnik, Technisches Englisch, Steuerungs- und Regelungstechnik, Vertiefungsprojekt, Allgemeine Betriebswirtschaftslehre, Qualitätsmanagement, CAD, Produktionstechnik, Integrierte Produktentwicklung, Wahlmodul, Finite Elemente Elastostatik, Maschinendynamik, Wahlmodul, Wahlmodul, Numerische Strömungsmechanik 1, Softwarebasierte Bauteilauslegung, Struktur- und Gestaltentwicklung, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Allgemeine Didaktik mit Eignungs- und Orientierungspraktikum, Auslandsaufenthalt, Berufspädagogik 1 und Berufsfeldpraktikum, Berufspädagogik 2, Diagnose und Förderung, Gender und Diversity: Erfolgsfaktoren
+für Unternehmen, International Activities , Technikdidaktik, Grundlagen Produktion und Logistik, Grundlagen Verfahrenstechnik, Informatik 1 - Imperative Programmierung, Informatik 2 - Objektorientierte Programmierung, Innovations- und Projektmanagement, Konstruieren mit Kunststoffen, Kreiselpumpen im Anlagenbau, Kunststoffverarbeitung, Lean Production, Leichtbauwerkstoffe, Thermodynamik der Energietechnik, Werkstoff- und Bauteilprüfung, Werkzeugmaschinen, Wärmeübertragung und Wärmespeicher</t>
+  </si>
+  <si>
+    <t>Materialtechnik</t>
+  </si>
+  <si>
+    <t>Einführung Maschinenbau, Festigkeitslehre, Mathematik 1, Statik, Technisches Zeichnen, Werkstofftechnik, Dynamik, Kunststofftechnik, Mathematik 2, Physik, Thermodynamik, Verbindungselemente, Basisprojekt, Getriebeelemente, Mathematik 3, Produktionstechnik, Prozess- und Informationsmanagement, Elektrische Maschinen, Strömungsmechanik, System- und Messtechnik, Technisches Englisch, Steuerungs- und Regelungstechnik, Vertiefungsprojekt, Allgemeine Betriebswirtschaftslehre, Qualitätsmanagement, Werkstoff- und Bauteilprüfung, Elektrische Maschinen, Kunststoffverarbeitung, Materialmodellierung und -simulation, Wahlmodul, Wahlmodul, Konstruieren mit Kunststoffen, Leichtbauwerkstoffe, Molekulare Werkstoffe, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Allgemeine Didaktik mit Eignungs- und Orientierungspraktikum, Auslandsaufenthalt, Berufspädagogik 1 und Berufsfeldpraktikum, Berufspädagogik 2, Diagnose und Förderung, Gender und Diversity: Erfolgsfaktoren
+für Unternehmen, International Activities , Technikdidaktik, Angewandte Produktion, Bildverarbeitung und Mustererkennung, Biochemie und Mikrobiologie, Chemie, Finite Elemente Elastostatik, Innovations- und Projektmanagement, Integrierte Produktentwicklung, Numerische Strömungsmechanik 1, Optische Technologien, Sensorik, Struktur- und Gestaltenentwicklung, Textile Technologien, Verfahrenstechnik, Werkzeugmaschinen, Wärmeübertragung und Wärmespeicher</t>
+  </si>
+  <si>
+    <t>Einführung in das Berufsfeld, Elektrotechnik 1, Grundlagen der Informatik, Mathematik 1, Physik, Digitaltechnik, Elektrotechnik 2, Mathematik 2, Objektorientierte Programmierung, Technische Mechanik - Statik und Festigkeitslehre, Elektrische Messtechnik, Halbleiterbauelemente und Schaltungen, Innovations- und Projektmanagement, Mathematik 3, Praxismodul 1, Technische Mechanik - Kinematik und Kinetik, Grundlagen der Kosntruktion, Industrielle Steuerungstechnik, Praxismodul 2, Regelungstechnik, Statistik, Datenbanken, Elektrische Maschinen, Technisches Englisch, Wahlmodul, Wahlmodul, Mechatronische Systeme 1, Mikrocontrollerprogrammierung, Praxismodul 3, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Antriebstechnik, Change Management, Data Analystics, Diagnose und Predictive Maintenance, Fertigungstechnik, Funktionale Sicherheit von Maschinen und Anlagen, Industrielle Kommunikation, Leistungselektronik, Messsysteme und Sensorik, Methodisches Konstruieren und CAD, Personal und Organisation, Qualitätsmanagement</t>
+  </si>
+  <si>
+    <t>Einführung in das Berufsfeld, Elektrotechnik 1, Grundlagen der Informatik, Mathematik 1, Physik, Digitaltechnik, Elektrotechnik 2, Mathematik 2, Objektorientierte Programmierung, Technische Mechanik - Statik und Festigkeitslehre, Elektrische Messtechnik, Halbleiterbauelemente und Schaltungen, Innovations- und Projektmanagement, Mathematik 3, Praxismodul 1, Technische Mechanik -  Kinematik und Kinetik, Grundlagen der Konstruktion, Industrielle Steuerungstechnik, Praxismodul 2, Regelungstechnik, Statistik, Datenbanken, Elektrische Maschinen, Technisches Englisch, Wahlmodul, Wahlmodul, Mechatronische Systeme 1, Mikrocontrollerprogrammierung, Praxismodul 3, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Antriebstechnik, Change Management, Data Analystics, Diagnose und Predictive Maintenance, Fertigungstechnik, Funktionale Sicherheit von Maschinen und Anlagen, Industrielle Kommunikation, Leistungselektronik, Messsysteme und Sensorik, Methodisches Konstruieren und CAD, Personald und Organisation, Qualitätsmanagement</t>
+  </si>
+  <si>
+    <t>Angewandte Mathematik</t>
+  </si>
+  <si>
+    <t>Analysis 1, Informatik, Lineare Algebra 1, Mathematische Ergänzung, Mathematische Modellierung praxisrelevanter Prozesse, Analysis 2, Betriebswirtschaft und Wirtschaftsmathematik, Englisch, Lineare Algebra 2, Objektorientierte Programmierung, Gewöhnliche Differentialgleichungen, Grundlagen Data Science, Interpolation und Approximation, Lineare Optimierung, Physikalisch-technische Anwendungen 1, Softwarelabor, Diskrete Mathematik, Grundlagen Produktion und Logistik, Numerik gewöhnlicher Differentialgleichungen, Numerische Mathematik, Physikalisch-technische Anwendungen 2, Stochastik, Künstliche Neuronale Netze, Maschinelles Lernen, Projektseminar (Angewandte Mathematik), Wahlmodul, Wahlmodul, Wahlmodul, Mathematisches Seminar, Nichtlineare Optimierung, Projekt Data Science, Wahlmodul, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Auslandsaufenthalt, Gender und Diversity: Erfolgsfaktoren für Unternehmen, International Activities, Akustische Signalverarbeitung in technischen und biologischen Systemen, Medizinische Bildgebungsverfahren, Digitale Fabrikplanung und Simulation, Operations Research, Spieltheorie, Datenbanken, Grundlagen der Kryptographie, Natural Language Processing, Predictive Analytics, Software Engineering</t>
+  </si>
+  <si>
+    <t>Auslandsaufenthalt, Gender und Diversity: Erfolgsfaktoren für Unternehmen, International Activities, Künstliche Neuronale Netze, Maschinelles Lernen, Digitale Fabrikplanung und Simulation, Operations Research, Spieltheorie, Aktuelle Themen der Medizintechnik, Biosignalverarbeitung und Neuroengineering, Biotechnologische Detektionssysteme, Biotechnologische Produktionsprozesse, Cooperative and Wearable Robotics, KI-basierte Medizinische Bildverarbeitung, Medizinische Datenverarbeitung, Neuroanatomie/-physiologie und Neurorehabilitation, Statistische Datenanalyse in Life Sciences</t>
+  </si>
+  <si>
+    <t>Auslandsaufenthalt, Gender und Diversity: Erfolgsfaktoren für Unternehmen, International Activities, Akustische Signalverarbeitung in technischen und biologischen Systemen, Medizinische Bildgebungsverfahren,  Künstliche Neuronale Netze, Maschinelles Lernen, Angewandte Produktion, Digitale Fabrikplanung und Simulation, Digitale Transformation von industriellen Unternehmensprozessen, Fabrikplanung, Lean Production, Personal und Organisation, Produktionsautomatisierung und -digitalisierung, Produktionsplanung und -steuerung, Produktionstechnik, Supply Chain Management, Unternehmensplanspiel Logistik oder General Management</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1171,6 +1512,53 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1205,16 +1593,49 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1517,8 +1938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1568,7 +1989,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,10 +2161,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G355"/>
+  <dimension ref="A1:G364"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1855,242 +2276,257 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>86</v>
       </c>
@@ -2532,12 +2968,12 @@
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>12</v>
+        <v>173</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>173</v>
+        <v>12</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
@@ -2735,82 +3171,88 @@
         <v>212</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B201" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B202" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>228</v>
       </c>
@@ -2975,82 +3417,85 @@
         <v>260</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B241" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>276</v>
       </c>
@@ -3161,7 +3606,7 @@
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278" t="s">
+      <c r="A278" s="13" t="s">
         <v>298</v>
       </c>
     </row>
@@ -3550,7 +3995,928 @@
         <v>375</v>
       </c>
     </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>384</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D21EA3-6A34-4B16-AF2A-5BAE175A5E61}">
+  <dimension ref="A1:F37"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" customWidth="1"/>
+    <col min="4" max="5" width="100.7109375" customWidth="1"/>
+    <col min="6" max="6" width="77.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="118.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="115.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>413</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>414</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="14" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="14" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="14" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>428</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>428</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>428</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>428</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>433</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>434</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="E27" s="7"/>
+    </row>
+    <row r="28" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>465</v>
+      </c>
+      <c r="B35" t="s">
+        <v>395</v>
+      </c>
+      <c r="C35" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>465</v>
+      </c>
+      <c r="B36" t="s">
+        <v>395</v>
+      </c>
+      <c r="C36" t="s">
+        <v>424</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>465</v>
+      </c>
+      <c r="B37" t="s">
+        <v>395</v>
+      </c>
+      <c r="C37" t="s">
+        <v>402</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>469</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="50a3624f-2342-413a-95f3-6f859866bf5a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008B46BE1F86C2D14EB496D3C1679E0290" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="21d0a59f2bb9451e1fe8c1c26106e08b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="50a3624f-2342-413a-95f3-6f859866bf5a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f5a8afb5de0b4bae4d84a45cae1589b" ns3:_="">
+    <xsd:import namespace="50a3624f-2342-413a-95f3-6f859866bf5a"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:_activity" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSystemTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="50a3624f-2342-413a-95f3-6f859866bf5a" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceDateTaken" ma:index="8" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="11" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="12" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_activity" ma:index="13" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSystemTags" ma:index="14" nillable="true" ma:displayName="MediaServiceSystemTags" ma:hidden="true" ma:internalName="MediaServiceSystemTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhaltstyp"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC65CAC6-5AA1-44DA-87CF-42367EE64157}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="50a3624f-2342-413a-95f3-6f859866bf5a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E44AFCBE-1BC5-408B-AE0A-65E369A63C51}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB9691BF-87DD-491D-B60E-5D5F923428FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="50a3624f-2342-413a-95f3-6f859866bf5a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added new questions and ects logic from datasource
</commit_message>
<xml_diff>
--- a/backend/zulassung.xlsx
+++ b/backend/zulassung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhbi-my.sharepoint.com/personal/steven_michel_fhbi_onmicrosoft_com/Documents/B.Eng/7. Semester/2. Innovations-&amp; Projektmanagement/Projektarbeit/HSBI_Chatbot/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="302" documentId="8_{9D362DC0-2740-4FD3-9197-17AC54460654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E53E7371-9A4E-450A-837E-726B6EDB8719}"/>
+  <xr:revisionPtr revIDLastSave="303" documentId="8_{9D362DC0-2740-4FD3-9197-17AC54460654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0D588F6-B920-457E-A2FC-BB51F988E096}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,9 +110,6 @@
     <t>Betriebswirtschaft</t>
   </si>
   <si>
-    <t xml:space="preserve">Modulbezeichnung </t>
-  </si>
-  <si>
     <t>Naturwissenschaft</t>
   </si>
   <si>
@@ -1494,6 +1491,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Modulbezeichnung</t>
   </si>
 </sst>
 </file>
@@ -2163,8 +2163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G364"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2180,7 +2180,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>470</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>10</v>
@@ -2189,7 +2189,7 @@
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>21</v>
@@ -2203,452 +2203,452 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F30" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F44" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F49" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F52" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F55" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
@@ -2658,317 +2658,317 @@
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
@@ -2978,1066 +2978,1066 @@
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B201" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B202" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B241" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -4064,19 +4064,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>386</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>387</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>388</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="135" x14ac:dyDescent="0.25">
@@ -4084,13 +4084,13 @@
         <v>19</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>390</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="10" t="s">
         <v>391</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>392</v>
       </c>
       <c r="E2" s="9"/>
     </row>
@@ -4099,16 +4099,16 @@
         <v>19</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>393</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="118.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -4116,16 +4116,16 @@
         <v>19</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="10" t="s">
         <v>397</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="115.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4133,16 +4133,16 @@
         <v>19</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>399</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>400</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -4150,16 +4150,16 @@
         <v>19</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>402</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>403</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -4167,518 +4167,518 @@
         <v>19</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>405</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>403</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D8" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>407</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>395</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="D9" s="10" t="s">
         <v>410</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>411</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D10" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>413</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>414</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>415</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>390</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>415</v>
-      </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>416</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>417</v>
       </c>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
+        <v>417</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>418</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>395</v>
-      </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>420</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>421</v>
       </c>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="14" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="14" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>395</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>396</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="14" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="14" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" s="10" t="s">
+        <v>427</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>428</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
+        <v>432</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>433</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>395</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>410</v>
-      </c>
-      <c r="D21" s="12" t="s">
+      <c r="E21" s="12" t="s">
         <v>434</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D22" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>436</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>396</v>
-      </c>
       <c r="D25" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>440</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C26" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>442</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>443</v>
       </c>
       <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C27" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>444</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>445</v>
       </c>
       <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>446</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>446</v>
-      </c>
-      <c r="D28" s="7" t="s">
+      <c r="E28" s="7" t="s">
         <v>447</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>449</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>402</v>
-      </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
         <v>450</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C30" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>452</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="E30" s="7" t="s">
         <v>453</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C31" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>455</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="E31" s="7" t="s">
         <v>456</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C32" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="D32" s="7" t="s">
         <v>458</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="E32" s="7" t="s">
         <v>459</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D33" s="7" t="s">
+        <v>460</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>461</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D34" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>463</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>464</v>
+      </c>
+      <c r="B35" t="s">
+        <v>394</v>
+      </c>
+      <c r="C35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="B35" t="s">
-        <v>395</v>
-      </c>
-      <c r="C35" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" s="3" t="s">
+      <c r="E35" s="3" t="s">
         <v>466</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>464</v>
+      </c>
+      <c r="B36" t="s">
+        <v>394</v>
+      </c>
+      <c r="C36" t="s">
+        <v>423</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="B36" t="s">
-        <v>395</v>
-      </c>
-      <c r="C36" t="s">
-        <v>424</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>466</v>
-      </c>
       <c r="E36" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>464</v>
+      </c>
+      <c r="B37" t="s">
+        <v>394</v>
+      </c>
+      <c r="C37" t="s">
+        <v>401</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="B37" t="s">
-        <v>395</v>
-      </c>
-      <c r="C37" t="s">
-        <v>402</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>466</v>
-      </c>
       <c r="E37" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
   </sheetData>
@@ -4687,23 +4687,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="50a3624f-2342-413a-95f3-6f859866bf5a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008B46BE1F86C2D14EB496D3C1679E0290" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="21d0a59f2bb9451e1fe8c1c26106e08b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="50a3624f-2342-413a-95f3-6f859866bf5a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f5a8afb5de0b4bae4d84a45cae1589b" ns3:_="">
     <xsd:import namespace="50a3624f-2342-413a-95f3-6f859866bf5a"/>
@@ -4885,25 +4868,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC65CAC6-5AA1-44DA-87CF-42367EE64157}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="50a3624f-2342-413a-95f3-6f859866bf5a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E44AFCBE-1BC5-408B-AE0A-65E369A63C51}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="50a3624f-2342-413a-95f3-6f859866bf5a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB9691BF-87DD-491D-B60E-5D5F923428FB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4919,4 +4901,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E44AFCBE-1BC5-408B-AE0A-65E369A63C51}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC65CAC6-5AA1-44DA-87CF-42367EE64157}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="50a3624f-2342-413a-95f3-6f859866bf5a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
get function get_vertiefungen_for more robust
</commit_message>
<xml_diff>
--- a/backend/zulassung.xlsx
+++ b/backend/zulassung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhbi-my.sharepoint.com/personal/steven_michel_fhbi_onmicrosoft_com/Documents/B.Eng/7. Semester/2. Innovations-&amp; Projektmanagement/Projektarbeit/HSBI_Chatbot/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="303" documentId="8_{9D362DC0-2740-4FD3-9197-17AC54460654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0D588F6-B920-457E-A2FC-BB51F988E096}"/>
+  <xr:revisionPtr revIDLastSave="309" documentId="8_{9D362DC0-2740-4FD3-9197-17AC54460654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48D0E697-C068-45C8-8F5A-B472596174CE}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="471">
   <si>
     <t>Schlüssel</t>
   </si>
@@ -2163,8 +2163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G364"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L94" sqref="L94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2611,82 +2611,100 @@
         <v>101</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G89" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G90" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G91" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G92" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G93" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G94" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>116</v>
       </c>
@@ -4687,6 +4705,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="50a3624f-2342-413a-95f3-6f859866bf5a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008B46BE1F86C2D14EB496D3C1679E0290" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="21d0a59f2bb9451e1fe8c1c26106e08b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="50a3624f-2342-413a-95f3-6f859866bf5a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f5a8afb5de0b4bae4d84a45cae1589b" ns3:_="">
     <xsd:import namespace="50a3624f-2342-413a-95f3-6f859866bf5a"/>
@@ -4868,24 +4903,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC65CAC6-5AA1-44DA-87CF-42367EE64157}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="50a3624f-2342-413a-95f3-6f859866bf5a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="50a3624f-2342-413a-95f3-6f859866bf5a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E44AFCBE-1BC5-408B-AE0A-65E369A63C51}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB9691BF-87DD-491D-B60E-5D5F923428FB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4901,22 +4937,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E44AFCBE-1BC5-408B-AE0A-65E369A63C51}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC65CAC6-5AA1-44DA-87CF-42367EE64157}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="50a3624f-2342-413a-95f3-6f859866bf5a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added dropout_rate in dashboard
</commit_message>
<xml_diff>
--- a/backend/zulassung.xlsx
+++ b/backend/zulassung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhbi-my.sharepoint.com/personal/steven_michel_fhbi_onmicrosoft_com/Documents/B.Eng/7. Semester/2. Innovations-&amp; Projektmanagement/Projektarbeit/HSBI_Chatbot/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="309" documentId="8_{9D362DC0-2740-4FD3-9197-17AC54460654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48D0E697-C068-45C8-8F5A-B472596174CE}"/>
+  <xr:revisionPtr revIDLastSave="798" documentId="8_{9D362DC0-2740-4FD3-9197-17AC54460654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC35CE96-DEC5-4118-8858-9F03CE393E01}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Allgemein" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="499">
   <si>
     <t>Schlüssel</t>
   </si>
@@ -119,6 +119,9 @@
     <t>Akustische Signalverarbeitung in technischen und biologischen Systemen</t>
   </si>
   <si>
+    <t>x</t>
+  </si>
+  <si>
     <t>Algorithmen und Datenstrukturen</t>
   </si>
   <si>
@@ -128,6 +131,9 @@
     <t>Allgemeine Didaktik</t>
   </si>
   <si>
+    <t>Allgemeine Didaktik mit Eignungs- und Orientierungspraktikum</t>
+  </si>
+  <si>
     <t>Allgemeine Volkswirtschaftslehre</t>
   </si>
   <si>
@@ -182,6 +188,9 @@
     <t>Berufspädagogik 1</t>
   </si>
   <si>
+    <t>Berufspädagogik 1 und Berufsfeldpraktikum</t>
+  </si>
+  <si>
     <t>Berufspädagogik 2</t>
   </si>
   <si>
@@ -311,7 +320,10 @@
     <t>Effiziente Lichttechnik</t>
   </si>
   <si>
-    <t>Einführug in das Berufsfeld (Digitale Technologien)</t>
+    <t>Einführung in das Berufsfeld Digitale Logistik</t>
+  </si>
+  <si>
+    <t>Einführung in das Berufsfeld (Digitale Technologien)</t>
   </si>
   <si>
     <t>Einführung in das Berufsfeld (MAT)</t>
@@ -869,13 +881,16 @@
     <t>Planung und Controlling</t>
   </si>
   <si>
-    <t>Prakikum Biotechnologie</t>
+    <t>Praktikum Biotechnologie 1</t>
   </si>
   <si>
     <t>Praktikum Biotechnologie 3</t>
   </si>
   <si>
-    <t>Praktium Biotechnologie 2</t>
+    <t>Praktikum Biotechnologie 2</t>
+  </si>
+  <si>
+    <t>Praxisprojekt Apparative Biotechnologie</t>
   </si>
   <si>
     <t>Predictive Analytics</t>
@@ -908,15 +923,24 @@
     <t>Programmierung autonomer Roboter</t>
   </si>
   <si>
+    <t>Projekt Apparative Biotechnologie</t>
+  </si>
+  <si>
     <t>Projekt Automatisierungstechnik</t>
   </si>
   <si>
     <t>Projekt Autonome Systeme und Robotik</t>
   </si>
   <si>
+    <t>Projekt Berufliche Bildung</t>
+  </si>
+  <si>
     <t>Projekt Data Science</t>
   </si>
   <si>
+    <t>Projekt Digitale Bahnsysteme</t>
+  </si>
+  <si>
     <t>Projekt Energie und Effizienz</t>
   </si>
   <si>
@@ -1010,6 +1034,9 @@
     <t>Software Engineering</t>
   </si>
   <si>
+    <t>Software Gruppenprojekt</t>
+  </si>
+  <si>
     <t>Softwarelabor</t>
   </si>
   <si>
@@ -1310,16 +1337,28 @@
     <t>Berufliche Bildung</t>
   </si>
   <si>
+    <t>Einführung in die Mechatronik, Elektrotechnik 1 - Gleichstromlehre, Informatik 1 - Imperative Programmierung, Konstruktion, Mathematik 1, Technische Mechanik 1, Elektrotechnik 2 - Wechselstromlehre, Informatik 2 - Objektorientierte Programmierung, Mathematik 2, Physikalische und messtechnische Grundlagen, Technische Mechanik 2, Werkstofftechnik, Grundlagen der Analog-und Digitalelektronik, Innovations- und Projektmanagement, Maschinenelemente, Mathematik 3, Regelungstechnik, Robotik - Einführung und Grundlagen, Eingebettete Systeme in der Mechatronik, Elektrische Antriebssysteme, Finite Elemente Methode, Sensor- und Aktorsysteme, Technisches Englisch, Verteilte Systeme, Allgemeine Didaktik mit Eignungs- und Orientierungspraktikum, Berufspädagogik 1 und Berufsfeldpraktikum, Diagnose und Förderung, Modellbildung und Simulation, Projekt Mechatronik, Wahlmodul, Allgemeine Betriebswirtschaftslehre, Berufspädagogik 2, Projekt Berufliche Bildung, Technikdidaktik, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
     <t>Akustische Signalverarbeitung in technischen und biologischen Systemen, Elektrotechnik 3, Feldsimulation, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Grundlagen Data Science, Integrierte Produktentwicklung, International Activities, Mess- und Prüfsysteme, Motion Control, Optische Technologien, Produktionstechnik, Projekt Mechatronik, Qualitätsmanagement, Rechnerarchitekturen, Signale und Systeme, Textile Technologies</t>
   </si>
   <si>
     <t>Medizintechnik</t>
   </si>
   <si>
+    <t>Einführung in die Mechatronik, Elektrotechnik 1 - Gleichstromlehre, Informatik 1 - Imperative Programmierung, Konstruktion, Mathematik 1, Technische Mechanik 1, Elektrotechnik 2 - Wechselstromlehre, Informatik 2 - Objektorientierte Programmierung, Mathematik 2, Physikalische und messtechnische Grundlagen, Technische Mechanik 2, Werkstofftechnik, Grundlagen der Analog-und Digitalelektronik, Innovations- und Projektmanagement, Maschinenelemente, Mathematik 3, Regelungstechnik, Robotik - Einführung und Grundlagen, Eingebettete Systeme in der Mechatronik, Elektrische Antriebssysteme, Finite Elemente Methode, Sensor- und Aktorsysteme, Technisches Englisch, Verteilte Systeme, Modellbildung und Simulation, Projekt Mechatronik, Wahlmodul, Wahlmodul, Wahlmodul, Wahlmodul, Allgemeine Betriebswirtschaftslehre, Wahlmodul, Wahlmodul, Wahlmodul, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
     <t>Akustische Signalverarbeitung in technischen und biologischen Systemen, Elektrotechnik 3, Feldsimulation, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Grundlagen Data Science, Integrierte Produktentwicklung, International Activities, Mess- und Prüfsysteme, Motion Control, Optische Technologien, Produktionstechnik, Projekt Mechatronik, Qualitätsmanagement, Rechnerarchitekturen, Signale und Systeme, Textile Technologies, Aktuelle Themen der Medizintechnik, Biosignalverarbeitung und Neuroengineering, Biotechnologische Detektionssysteme, Biotechnologische Produktionsprozesse, Cooperative and Wearable Robotics, KI-basierte Medizinische Bildverarbeitung, Medizinische Bildgebungsverfahren, Medizinische Datenverarbeitung, Neuroanatomie/-physiologie und Neurorehabilitation, Projekt Medizintechnik</t>
   </si>
   <si>
+    <t>Einführung in die Mechatronik, Elektrotechnik 1 - Gleichstromlehre, Informatik 1 - Imperative Programmierung, Konstruktion, Mathematik 1, Technische Mechanik 1, Elektrotechnik 2 - Wechselstromlehre, Informatik 2 - Objektorientierte Programmierung, Mathematik 2, Physikalische und messtechnische Grundlagen, Technische Mechanik 2, Werkstofftechnik, Grundlagen der Analog-und Digitalelektronik, Innovations- und Projektmanagement, Maschinenelemente, Mathematik 3, Regelungstechnik, Robotik - Einführung und Grundlagen, Eingebettete Systeme in der Mechatronik, Elektrische Antriebssysteme, Finite Elemente Methode, Sensor- und Aktorsysteme, Technisches Englisch, Verteilte Systeme, Fahrzeugdynamik, Modellbildung und Simulation, Projekt Mechanik, Schienenfahrzeugtechnik, Wahlmodul, Wahlmodul, Allgemeine Betriebswirtschaftslehre, Fahrassistenzsysteme und automatisiertes Fahren, Projekt Mobilität, Wahlmodul, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
     <t>Akustische Signalverarbeitung in technischen und biologischen Systemen, Elektrotechnik 3, Feldsimulation, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Grundlagen Data Science, Integrierte Produktentwicklung, International Activities, Mess- und Prüfsysteme, Motion Control, Optische Technologien, Produktionstechnik, Projekt Mechatronik, Qualitätsmanagement, Rechnerarchitekturen, Signale und Systeme, Textile Technologies, Einführung System Bahn, Electromobility, Mikromobilität, Optische Systeme in mobilen und autonomen Anwendungen, Sensorik, Verkehrswirtschaft</t>
+  </si>
+  <si>
+    <t>Einführung in die Mechatronik, Elektrotechnik 1 - Gleichstromlehre, Informatik 1 - Imperative Programmierung, Konstruktion, Mathematik 1, Technische Mechanik 1, Elektrotechnik 2 - Wechselstromlehre, Informatik 2 - Objektorientierte Programmierung, Mathematik 2, Physikalische und messtechnische Grundlagen, Technische Mechanik 2, Werkstofftechnik, Grundlagen der Analog-und Digitalelektronik, Innovations- und Projektmanagement, Maschinenelemente, Mathematik 3, Regelungstechnik, Robotik - Einführung und Grundlagen, Eingebettete Systeme in der Mechatronik, Elektrische Antriebssysteme, Finite Elemente Methode, Sensor- und Aktorsysteme, Technisches Englisch, Verteilte Systeme, Modellbildung und Simulation, Projekt Mechatronik, Projekt Nachhaltige Produkte und Prozesse, Wahlmodul, Zirkuläre Wertschöpfung, Allgemeine Betriebswirtschaftslehre, Integrierte Produktentwicklung, Nachhaltigkeitsbewertung und -analyse, Wahlmodul, Wahlmodul, Wahlmodul</t>
   </si>
   <si>
     <t>Akustische Signalverarbeitung in technischen und biologischen Systemen, Elektrotechnik 3, Feldsimulation, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Grundlagen Data Science, Integrierte Produktentwicklung, International Activities, Mess- und Prüfsysteme, Motion Control, Optische Technologien, Produktionstechnik, Projekt Mechatronik, Qualitätsmanagement, Rechnerarchitekturen, Signale und Systeme, Textile Technologies, Electromobility, Energiemanagement, Nachhaltige Gebäude, Photovoltaik, Produkt-Risikomanagement, Sensorik, Thermische Nutzung regenerativer Energien, Wind- und Wasserkraft</t>
@@ -1341,9 +1380,6 @@
   <si>
     <t xml:space="preserve">Aktuelle Themen der Medizintechnik, Ambient Assisted Living, Auslandsaufenthalt, Cooperative and Wearable Robotics, Electronic Marketing, Elektrotechnik 3, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Grundlagen Data Science, Grundlagen der Kryptographie, Integrierte Produktentwicklung, International Activities, Internationales Marketing, Internes Rechnungswesen, Investition und Finanzierung, KI-basierte Medizinische Bildverarbeitung, Künstliche Neuronale Netze, Maschinelles Lernen, Medizinische Bildgebungsverfahren, Medizinische Datenverarbeitung, Messtechnik, Mikrosystemtechnik, Motion Control, Natural Language Processing, Optoelektronik, Personal und Organisation, Qualitätsmanagement, Robotik - Einführung und Grundlagen, Sensor- und Aktorsysteme, Sensorik, Signale und Systeme, Stochastik, Technisches Englisch 2, Theoretische Informatik, Vernetzte Systeme mit Mikrocontrollern, Web-Technologien 1, Web-Technologien 2, Diskrete Mathematik, Grundlagen der Kryptographie, Predictive Analytics, Stochastik
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elektotechnik </t>
   </si>
   <si>
     <t>Elektrotechnik 1, Informatik 1, Ingenieurmathematik 1, Physik 1, Werkstoffe der Elektrotechnik und
@@ -1490,10 +1526,59 @@
     <t>Auslandsaufenthalt, Gender und Diversity: Erfolgsfaktoren für Unternehmen, International Activities, Akustische Signalverarbeitung in technischen und biologischen Systemen, Medizinische Bildgebungsverfahren,  Künstliche Neuronale Netze, Maschinelles Lernen, Angewandte Produktion, Digitale Fabrikplanung und Simulation, Digitale Transformation von industriellen Unternehmensprozessen, Fabrikplanung, Lean Production, Personal und Organisation, Produktionsautomatisierung und -digitalisierung, Produktionsplanung und -steuerung, Produktionstechnik, Supply Chain Management, Unternehmensplanspiel Logistik oder General Management</t>
   </si>
   <si>
-    <t>x</t>
+    <t>Apparative Biotechnologie</t>
+  </si>
+  <si>
+    <t>Chemie, Elektrotechnik 1 - Gleichstromlehre, Informatik 1 - Imperative Programmierung, Mathematik 1, Molekularbiologie der Zelle, Technische Mechanik, Biotechnologie 1, Elektrotechnik 2 - Wechselstromlehre, Konstruktion, Mathematik 2, Physikalische und messtechnische Grundlagen, Praktikum Biotechnologie 1, Biotechnologie 2, Chemie 2, Innovations- und Projektmanagement, Praktikum Biotechnologie 2, Projekt Apparative Biotechnologie,  Regelungstechnik, Allgemeine Betriebswirtschaftslehre, Biotechnologie 3, Praktikum Biotechnologie 3, Praxisprojekt Apparative Biotechnologie, Sensor- und Aktorsysteme, Technisches Englisch, Angewandte Biotechnologie, Biotechnologische Detektionssysteme, Produktaufreinigung, Projekt Nachhaltige Produkte und Prozesse, Zirkuläre Wertschöpfung, Nachhaltigkeitsbewertung und -analyse, Wahlmodul, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Auslandsaufenthalt, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Individuelle Profilbildung, International Activities, Praxisphase, Electromobility, Energiemanagement, Integrierte Produktentwicklung, Nachhaltige Gebäude, Photovoltaik, Produkt-Risikomanagement, Sensorik, Thermische Nutzung regenerativer Energien, Wind- und Wasserkraft</t>
+  </si>
+  <si>
+    <t>Chemie, Elektrotechnik 1 - Gleichstromlehre, Informatik 1 - Imperative Programmierung, Mathematik 1, Molekularbiologie der Zelle, Technische Mechanik, Biotechnologie 1, Elektrotechnik 2 - Wechselstromlehre, Konstruktion, Mathematik 2, Physikalische und messtechnische Grundlagen, Praktikum Biotechnologie 1, Biotechnologie 2, Chemie 2, Innovations- und Projektmanagement, Praktikum Biotechnologie 2, Projekt Apparative Biotechnologie,  Regelungstechnik, Allgemeine Betriebswirtschaftslehre, Biotechnologie 3, Praktikum Biotechnologie 3, Praxisprojekt Apparative Biotechnologie, Sensor- und Aktorsysteme, Technisches Englisch, Angewandte Biotechnologie, Biotechnologische Detektionssysteme, Produktaufreinigung, Wahlmodul, Wahlmodul, Wahlmodul, Wahlmodul, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Auslandsaufenthalt, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Individuelle Profilbildung, International Activities, Praxisphase, Biotechnologische Detektionssysteme, Biotechnologische Produktionsprozesse, Mess- und Prüfsysteme, Modellbildung und Simulation, Motion Control, Predictive Analytics, Projekt Automatisierungstechnik, Vernetzte Systeme mit Mikrocontrollern, Zustandsbeobachtung und -schätzung, Zustandsregelungen</t>
+  </si>
+  <si>
+    <t>Auslandsaufenthalt, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Individuelle Profilbildung, International Activities, Praxisphase,  Aktuelle Themen der Medizintechnik, Akustische Signalverarbeitung in technischen und biologischen Systemen, Biosignalverarbeitung und Neuroengineering, Biotechnologische Detektionssysteme, Biotechnologische Produktionsprozesse, Cooperative and Wearable Robotics, KI-basierte Medizinische Bildverarbeitung, Medizinische Bildgebungsverfahren, Medizinische Datenverarbeitung, Neuroanatomie/-physiologie und Neurorehabilitation, Projekt Medizintechnik</t>
+  </si>
+  <si>
+    <t>Chemie, Elektrotechnik 1 - Gleichstromlehre, Informatik 1 - Imperative Programmierung, Mathematik 1, Molekularbiologie der Zelle, Technische Mechanik, Biotechnologie 1, Elektrotechnik 2 - Wechselstromlehre, Konstruktion, Mathematik 2, Physikalische und messtechnische Grundlagen, Praktikum Biotechnologie 1, Biotechnologie 2, Chemie 2, Innovations- und Projektmanagement, Praktikum Biotechnologie 2, Projekt Apparative Biotechnologie,  Regelungstechnik, Allgemeine Betriebswirtschaftslehre, Biotechnologie 3, Praktikum Biotechnologie 3, Praxisprojekt Apparative Biotechnologie, Sensor- und Aktorsysteme, Technisches Englisch, Angewandte Biotechnologie, Biotechnologische Detektionssysteme, Produktaufreinigung, Biotechnologische Produktionsprozesse, Integrierte Produktentwicklung,  Wahlmodul, Wahlmodul, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Auslandsaufenthalt, Gender und Diversity: Erfolgsfaktoren für Unternehmen, Individuelle Profilbildung, International Activities, Praxisphase,</t>
+  </si>
+  <si>
+    <t>Digitale Bahnsysteme</t>
+  </si>
+  <si>
+    <t>Einführung System Bahn, Elektrotechnik, Grundlagen der Informatik, Mathematik 1, Naturwissenschaftliche Grundlagen, Technische Mechanik 1, Fahrzeugtechnik, Mathematik 2, Messtechnik, Objektorientierte Programmierung, Technische Mechanik 2, Technisches Englisch, Betriebswirtschaftslehre, Eisenbahninfrastruktur (Fahrweg Leit- und Sicherungstechnik), Kommunikationstechnik, Numerische Mathematik, Sensorik und Aktorik, Software Engineering, Logistik und Verkehrssysteme, Maschinen- und Systemdynamik, Modellbildung und Simulation, Projekt Digitale Bahnsysteme, Projekt Digitale Bahnsysteme, Signale und Systeme, Software Gruppenprojekt, Grundlagen Maschinelles Lernen, Grundlagen der Bildverarbeitung, Projektmanagement, Regelungstechnik, Zulassung und Recht formelle Randbedingungen Eisenbahnbetrieb</t>
+  </si>
+  <si>
+    <t>Digitale Logistik</t>
+  </si>
+  <si>
+    <t>Praxisintegriert</t>
+  </si>
+  <si>
+    <t>Einführung in das Berufsfeld Digitale Logistik, Grundlagen der Programmierung, Grundlagen der Wirtschaftswissenschaften, Mathematik 1, Technische Grundlagen, Beschaffung Produktion und Logistik, Datenbanken, Materialflusstechnik, Operations Research, Rechnungswesen Investition Finanzierung und Steuern, Geschäftsprozessmodellierung und IT-Systeme, Innovations- und Projektmanagement, Statistik, Technisches Englisch, Verpackungstechnik und Ladungssicherung, Digital Service Engineering und Dienstleistungsmarketing, Lean Production, Logistische IT-Systeme, Qualitätsmanagement, Web-Technologien, Business Intelligence, Data Analytics, Cyberphysische Logistiksysteme, Mikrocontrollerprogrammierung, Personal und Organisation, Transport- Speditions- Zoll- und Außenhandelsrecht, Wahlmodul, Wahlmodul, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Digitale Fabrikplanung und Simulation, Identifikationssysteme, Industrial Engineering, Interkulturelle Kommunikation, Produktionsplanung und -steuerung, Supply Chain Management, Transportlogistik, Verteil- und Sortiersysteme</t>
+  </si>
+  <si>
+    <t>Grundlagen der Betriebswirtschaftslehre, Grundlagen der Informatik, Grundlagen von Data Science und Datenschutz, Mathematik 1, Technisches Englisch, Data Mining, Datenbanken, Mathematik 2, Objektorientierte Programmierung, Statistik, Big Data, HMI und Bedienoberflächen, Mathematik 3, Vernetzung und IoT-Lösungen, Algorithmen und Datenstrukturen, Innovations- und Projektmanagement, Maschinelles Lernen, Operations Research, Web-Technologien, Geschäftsprozessmodellierung und IT-Systeme, Software Engineering, Sprach- und Bilderkennung, Assistenzsysteme, Safety und Security, Cluster Computing, Qualitätssicherung für KI-Systeme, Wahlmodul, Wahlmodul, Wahlmodul, Wahlmodul</t>
+  </si>
+  <si>
+    <t>Change Management, Diagnose und Predictive Maintenance, Digitale Geschäftsmodelle und Wertschöpfungsketten, Industrielle Steuerungstechnik, Marketing und Technischer Vertrieb, Sensorik und Aktorik, Smart Services und Devices, Social Media and Natural Language
+Processing</t>
   </si>
   <si>
     <t>Modulbezeichnung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elektrotechnik </t>
   </si>
 </sst>
 </file>
@@ -1561,12 +1646,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1597,7 +1688,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1632,6 +1723,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1989,7 +2084,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,10 +2256,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G364"/>
+  <dimension ref="A1:R372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L94" sqref="L94"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2176,11 +2271,17 @@
     <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" customWidth="1"/>
+    <col min="16" max="16" width="18" customWidth="1"/>
+    <col min="17" max="17" width="14.5703125" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>470</v>
+        <v>497</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>10</v>
@@ -2202,7 +2303,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2210,1852 +2311,2180 @@
       <c r="A3" t="s">
         <v>24</v>
       </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
+      <c r="A6" s="15" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>28</v>
+      <c r="A7" s="15" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="G19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="F20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="G21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="G22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="E28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="F29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>51</v>
-      </c>
-      <c r="F30" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="E30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="E31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="F32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="F33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="D34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="G35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="D36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="D37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="D38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="G39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="E40" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="F41" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="F42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="E43" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>65</v>
-      </c>
-      <c r="F44" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="D44" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="D45" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="F46" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="E47" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="G48" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F49" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="F50" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="F51" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F52" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="F53" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="F54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>76</v>
-      </c>
-      <c r="F55" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="M56" s="16"/>
+      <c r="N56" s="16"/>
+      <c r="O56" s="16"/>
+      <c r="P56" s="16"/>
+      <c r="Q56" s="16"/>
+      <c r="R56" s="16"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="F57" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="E58" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="F59" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="E60" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="E61" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="E62" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="F63" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="F64" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="G65" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="B66" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="D67" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="E68" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="G69" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="15" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="15" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="F74" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="F75" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="G76" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="D77" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="G78" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="C79" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>101</v>
+        <v>102</v>
+      </c>
+      <c r="G80" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>102</v>
+        <v>103</v>
+      </c>
+      <c r="G81" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>103</v>
+        <v>104</v>
+      </c>
+      <c r="E82" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="G83" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>105</v>
+        <v>106</v>
+      </c>
+      <c r="G84" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>106</v>
+        <v>107</v>
+      </c>
+      <c r="G85" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>107</v>
+        <v>108</v>
+      </c>
+      <c r="G86" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+      <c r="G87" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>109</v>
+        <v>110</v>
+      </c>
+      <c r="G88" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>13</v>
+        <v>111</v>
       </c>
       <c r="G89" t="s">
-        <v>469</v>
+        <v>25</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G90" t="s">
-        <v>469</v>
+        <v>25</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G91" t="s">
-        <v>469</v>
+        <v>25</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>112</v>
+        <v>13</v>
       </c>
       <c r="G92" t="s">
-        <v>469</v>
+        <v>25</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G93" t="s">
-        <v>469</v>
+        <v>25</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G94" t="s">
-        <v>469</v>
+        <v>25</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>115</v>
+        <v>116</v>
+      </c>
+      <c r="G95" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="G96" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="G97" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="F98" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="E99" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="E100" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="G101" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A102" s="15" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A103" s="15" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A104" s="15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="G105" t="s">
+        <v>25</v>
+      </c>
+      <c r="L105" s="16"/>
+      <c r="M105" s="16"/>
+      <c r="N105" s="16"/>
+      <c r="O105" s="16"/>
+      <c r="P105" s="16"/>
+      <c r="Q105" s="16"/>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="E106" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="E107" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="E108" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G109" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A110" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="G111" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="D112" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="D113" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="D114" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="D115" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="B116" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="G117" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G118" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="D120" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="F121" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="D122" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="B123" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="F124" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>12</v>
+        <v>174</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>175</v>
+        <v>12</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>220</v>
-      </c>
-      <c r="B201" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>221</v>
-      </c>
-      <c r="B202" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>260</v>
-      </c>
-      <c r="B241" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A262" t="s">
-        <v>281</v>
+      <c r="A262" s="13" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A273" t="s">
-        <v>292</v>
+      <c r="A273" s="13" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278" s="13" t="s">
-        <v>297</v>
+      <c r="A278" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285" t="s">
-        <v>304</v>
+      <c r="A285" s="13" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>383</v>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -4065,10 +4494,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D21EA3-6A34-4B16-AF2A-5BAE175A5E61}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4082,19 +4511,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="135" x14ac:dyDescent="0.25">
@@ -4102,13 +4531,13 @@
         <v>19</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="E2" s="9"/>
     </row>
@@ -4117,16 +4546,16 @@
         <v>19</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="118.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -4134,16 +4563,16 @@
         <v>19</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="115.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4151,16 +4580,16 @@
         <v>19</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -4168,16 +4597,16 @@
         <v>19</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -4185,518 +4614,633 @@
         <v>19</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>421</v>
-      </c>
-      <c r="D13" s="9"/>
+        <v>430</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>431</v>
+      </c>
       <c r="E13" s="14" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="D14" s="9"/>
+        <v>433</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>434</v>
+      </c>
       <c r="E14" s="14" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>395</v>
-      </c>
-      <c r="D15" s="9"/>
+        <v>404</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>436</v>
+      </c>
       <c r="E15" s="14" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>398</v>
-      </c>
-      <c r="D16" s="9"/>
+        <v>407</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>438</v>
+      </c>
       <c r="E16" s="14" t="s">
-        <v>426</v>
+        <v>439</v>
       </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>427</v>
+        <v>440</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>428</v>
+        <v>441</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>427</v>
+        <v>440</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>429</v>
+        <v>442</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>427</v>
+        <v>440</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>430</v>
+        <v>443</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>427</v>
+        <v>440</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>431</v>
+        <v>444</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>432</v>
+        <v>498</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>433</v>
+        <v>445</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>434</v>
+        <v>446</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>432</v>
+        <v>498</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>436</v>
+        <v>448</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>432</v>
+        <v>498</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>432</v>
+        <v>498</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>432</v>
+        <v>498</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>439</v>
+        <v>451</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>440</v>
+        <v>452</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>432</v>
+        <v>498</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>441</v>
+        <v>453</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>442</v>
+        <v>454</v>
       </c>
       <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>432</v>
+        <v>498</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>443</v>
+        <v>455</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>444</v>
+        <v>456</v>
       </c>
       <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>446</v>
+        <v>458</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>447</v>
+        <v>459</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>451</v>
+        <v>463</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>452</v>
+        <v>464</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>454</v>
+        <v>466</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>455</v>
+        <v>467</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>456</v>
+        <v>468</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>457</v>
+        <v>469</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>460</v>
+        <v>472</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>461</v>
+        <v>473</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>462</v>
+        <v>474</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>463</v>
+        <v>475</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>464</v>
+        <v>476</v>
       </c>
       <c r="B35" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C35" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>465</v>
+        <v>477</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>466</v>
+        <v>478</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>464</v>
+        <v>476</v>
       </c>
       <c r="B36" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C36" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>465</v>
+        <v>477</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>467</v>
+        <v>479</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>464</v>
+        <v>476</v>
       </c>
       <c r="B37" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C37" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>465</v>
+        <v>477</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>468</v>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>481</v>
+      </c>
+      <c r="B38" t="s">
+        <v>403</v>
+      </c>
+      <c r="C38" t="s">
+        <v>407</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>481</v>
+      </c>
+      <c r="B39" t="s">
+        <v>403</v>
+      </c>
+      <c r="C39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>481</v>
+      </c>
+      <c r="B40" t="s">
+        <v>403</v>
+      </c>
+      <c r="C40" t="s">
+        <v>433</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>481</v>
+      </c>
+      <c r="B41" t="s">
+        <v>403</v>
+      </c>
+      <c r="C41" t="s">
+        <v>481</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>489</v>
+      </c>
+      <c r="B42" t="s">
+        <v>403</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>491</v>
+      </c>
+      <c r="B43" t="s">
+        <v>492</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" t="s">
+        <v>492</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>496</v>
       </c>
     </row>
   </sheetData>
@@ -4705,23 +5249,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="50a3624f-2342-413a-95f3-6f859866bf5a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008B46BE1F86C2D14EB496D3C1679E0290" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="21d0a59f2bb9451e1fe8c1c26106e08b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="50a3624f-2342-413a-95f3-6f859866bf5a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f5a8afb5de0b4bae4d84a45cae1589b" ns3:_="">
     <xsd:import namespace="50a3624f-2342-413a-95f3-6f859866bf5a"/>
@@ -4903,25 +5430,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC65CAC6-5AA1-44DA-87CF-42367EE64157}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="50a3624f-2342-413a-95f3-6f859866bf5a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E44AFCBE-1BC5-408B-AE0A-65E369A63C51}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="50a3624f-2342-413a-95f3-6f859866bf5a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB9691BF-87DD-491D-B60E-5D5F923428FB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4937,4 +5463,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E44AFCBE-1BC5-408B-AE0A-65E369A63C51}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC65CAC6-5AA1-44DA-87CF-42367EE64157}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="50a3624f-2342-413a-95f3-6f859866bf5a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>